<commit_message>
after 8 month try to run
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/OpenCartTestData.xlsx
+++ b/src/test/resources/testdata/OpenCartTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Acceleration\workspace\Aug2023POMSeries\src\test\resources1\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Acceleration\workspace\Aug2023POMSeries\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427C4EFE-05F0-4E37-B2D0-3D949BD2F53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CE2FBB-B926-4AD8-BE2F-C3A750ADA8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7395" yWindow="2145" windowWidth="12720" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
@@ -485,7 +485,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="A1:E4"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +580,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="A1:C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>